<commit_message>
modified:   perfood tables/Monthly_Sales_Parts_Per_Item.xlsx 	new file:   perweek 6pm/RFaktors.xlsx 	new file:   perweek 6pm/RSefaresh.xlsx 	new file:   perweek 6pm/Rfakitm.xlsx 	new file:   perweek 6pm/Sales_Per_Item_Day_Time_New.xlsx 	new file:   perweek 6pm/main.py 	modified:   weekday and monthly analysis/Monthly_Sales_Parts_Persian.xlsx 	new file:   weekday and monthly analysis/Total_Price_Per_Item_Day.xlsx 	modified:   weekday and monthly analysis/Weekly_Sales_Per_Day.xlsx 	modified:   weekday and monthly analysis/main.py 	new file:   weekday and monthly analysis/main_weekdays.py
</commit_message>
<xml_diff>
--- a/perfood tables/Monthly_Sales_Parts_Per_Item.xlsx
+++ b/perfood tables/Monthly_Sales_Parts_Per_Item.xlsx
@@ -5,17 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhshi\Videos\snapp_box_integration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhshi\Videos\Restaurant_data_analysis\perfood tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8794A37-E08C-4D48-ABEA-56CF085FA2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2982512-DCF1-4A72-A8EC-60266A3094CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -666,7 +678,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -717,136 +731,136 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>3655000</v>
+        <v>8000</v>
       </c>
       <c r="C4">
-        <v>4084000</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>5032000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B5">
-        <v>1180000</v>
+        <v>291000</v>
       </c>
       <c r="C5">
-        <v>1562500</v>
+        <v>43000</v>
       </c>
       <c r="D5">
-        <v>1852500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B6">
-        <v>220000</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>386000</v>
+        <v>400000</v>
       </c>
       <c r="D6">
-        <v>358000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B7">
-        <v>448000</v>
+        <v>37000</v>
       </c>
       <c r="C7">
-        <v>473000</v>
+        <v>64000</v>
       </c>
       <c r="D7">
-        <v>392000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="B8">
-        <v>13058000</v>
+        <v>150000</v>
       </c>
       <c r="C8">
-        <v>11589000</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>11844000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B9">
-        <v>39934000</v>
+        <v>6000</v>
       </c>
       <c r="C9">
-        <v>38194000</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>39205000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="B10">
-        <v>2464000</v>
+        <v>30000</v>
       </c>
       <c r="C10">
-        <v>2108000</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>2116000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B11">
-        <v>11656000</v>
+        <v>48000</v>
       </c>
       <c r="C11">
-        <v>11001000</v>
+        <v>45000</v>
       </c>
       <c r="D11">
-        <v>12364000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="B12">
-        <v>925000</v>
+        <v>92000</v>
       </c>
       <c r="C12">
-        <v>845000</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1005000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="B13">
-        <v>8000</v>
+        <v>60000</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -857,394 +871,394 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="B14">
+        <v>6000</v>
+      </c>
+      <c r="C14">
         <v>15000</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
       <c r="D14">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="B15">
-        <v>7248000</v>
+        <v>10000</v>
       </c>
       <c r="C15">
-        <v>3889000</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>6227000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="B16">
-        <v>1393000</v>
+        <v>14500</v>
       </c>
       <c r="C16">
-        <v>1776000</v>
+        <v>11000</v>
       </c>
       <c r="D16">
-        <v>1120000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B17">
-        <v>1050000</v>
+        <v>6000</v>
       </c>
       <c r="C17">
-        <v>260000</v>
+        <v>1500</v>
       </c>
       <c r="D17">
-        <v>260000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>1875000</v>
+        <v>15000</v>
       </c>
       <c r="C18">
-        <v>1385000</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>1490000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="B19">
-        <v>39003000</v>
+        <v>16500</v>
       </c>
       <c r="C19">
-        <v>41119000</v>
+        <v>37500</v>
       </c>
       <c r="D19">
-        <v>40209000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B20">
-        <v>5353000</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>6744000</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>5215000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B21">
-        <v>5210000</v>
+        <v>135000</v>
       </c>
       <c r="C21">
-        <v>4286000</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>4105000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="B22">
-        <v>25182000</v>
+        <v>132000</v>
       </c>
       <c r="C22">
-        <v>24248000</v>
+        <v>198000</v>
       </c>
       <c r="D22">
-        <v>24172000</v>
+        <v>88000</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B23">
-        <v>824000</v>
+        <v>69000</v>
       </c>
       <c r="C23">
-        <v>1314000</v>
+        <v>67000</v>
       </c>
       <c r="D23">
-        <v>865000</v>
+        <v>96000</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="B24">
-        <v>10682000</v>
+        <v>132000</v>
       </c>
       <c r="C24">
-        <v>9214000</v>
+        <v>181500</v>
       </c>
       <c r="D24">
-        <v>8703000</v>
+        <v>115500</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B25">
-        <v>2209000</v>
+        <v>72000</v>
       </c>
       <c r="C25">
-        <v>1515000</v>
+        <v>105000</v>
       </c>
       <c r="D25">
-        <v>1388000</v>
+        <v>164000</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B26">
-        <v>5401000</v>
+        <v>62500</v>
       </c>
       <c r="C26">
-        <v>5642000</v>
+        <v>500000</v>
       </c>
       <c r="D26">
-        <v>4642000</v>
+        <v>187500</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B27">
-        <v>291000</v>
+        <v>375000</v>
       </c>
       <c r="C27">
-        <v>43000</v>
+        <v>375000</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B28">
-        <v>21522000</v>
+        <v>273000</v>
       </c>
       <c r="C28">
-        <v>18687000</v>
+        <v>231000</v>
       </c>
       <c r="D28">
-        <v>20505000</v>
+        <v>252000</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B29">
-        <v>69000</v>
+        <v>1050000</v>
       </c>
       <c r="C29">
-        <v>67000</v>
+        <v>260000</v>
       </c>
       <c r="D29">
-        <v>96000</v>
+        <v>260000</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>275000</v>
       </c>
       <c r="C30">
-        <v>400000</v>
+        <v>365000</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B31">
-        <v>37000</v>
+        <v>240000</v>
       </c>
       <c r="C31">
-        <v>64000</v>
+        <v>480000</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B32">
-        <v>12683000</v>
+        <v>220000</v>
       </c>
       <c r="C32">
-        <v>13015000</v>
+        <v>386000</v>
       </c>
       <c r="D32">
-        <v>13890000</v>
+        <v>358000</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B33">
-        <v>3261000</v>
+        <v>730000</v>
       </c>
       <c r="C33">
-        <v>2840000</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>1742000</v>
+        <v>390000</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B34">
-        <v>1536000</v>
+        <v>448000</v>
       </c>
       <c r="C34">
-        <v>2122200</v>
+        <v>473000</v>
       </c>
       <c r="D34">
-        <v>1822200</v>
+        <v>392000</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B35">
-        <v>273000</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>231000</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>252000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B36">
-        <v>788640</v>
+        <v>420000</v>
       </c>
       <c r="C36">
-        <v>906180</v>
+        <v>525000</v>
       </c>
       <c r="D36">
-        <v>916680</v>
+        <v>420000</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B37">
-        <v>450000</v>
+        <v>190000</v>
       </c>
       <c r="C37">
-        <v>500000</v>
+        <v>220000</v>
       </c>
       <c r="D37">
-        <v>500000</v>
+        <v>495000</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38">
-        <v>62500</v>
+        <v>450000</v>
       </c>
       <c r="C38">
         <v>500000</v>
       </c>
       <c r="D38">
-        <v>187500</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="B39">
-        <v>375000</v>
+        <v>2270000</v>
       </c>
       <c r="C39">
-        <v>375000</v>
+        <v>1605000</v>
       </c>
       <c r="D39">
-        <v>250000</v>
+        <v>555000</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B40">
-        <v>1320000</v>
+        <v>400000</v>
       </c>
       <c r="C40">
-        <v>1600000</v>
+        <v>240000</v>
       </c>
       <c r="D40">
-        <v>1822000</v>
+        <v>560000</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B41">
-        <v>3048000</v>
+        <v>899000</v>
       </c>
       <c r="C41">
-        <v>5020000</v>
+        <v>606000</v>
       </c>
       <c r="D41">
-        <v>5242000</v>
+        <v>570000</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1263,691 +1277,694 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B43">
-        <v>150000</v>
+        <v>480000</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>240000</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>715000</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B44">
-        <v>6000</v>
+        <v>824000</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1314000</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>865000</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B45">
-        <v>2249400</v>
+        <v>673000</v>
       </c>
       <c r="C45">
-        <v>2414600</v>
+        <v>879000</v>
       </c>
       <c r="D45">
-        <v>1557600</v>
+        <v>911000</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B46">
-        <v>994500</v>
+        <v>788640</v>
       </c>
       <c r="C46">
-        <v>977000</v>
+        <v>906180</v>
       </c>
       <c r="D46">
-        <v>1290500</v>
+        <v>916680</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B47">
-        <v>480000</v>
+        <v>702300</v>
       </c>
       <c r="C47">
-        <v>240000</v>
+        <v>852500</v>
       </c>
       <c r="D47">
-        <v>715000</v>
+        <v>966600</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B48">
-        <v>132000</v>
+        <v>925000</v>
       </c>
       <c r="C48">
-        <v>198000</v>
+        <v>845000</v>
       </c>
       <c r="D48">
-        <v>88000</v>
+        <v>1005000</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B49">
-        <v>899000</v>
+        <v>1393000</v>
       </c>
       <c r="C49">
-        <v>606000</v>
+        <v>1776000</v>
       </c>
       <c r="D49">
-        <v>570000</v>
+        <v>1120000</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B50">
-        <v>2794000</v>
+        <v>734250</v>
       </c>
       <c r="C50">
-        <v>2262000</v>
+        <v>800250</v>
       </c>
       <c r="D50">
-        <v>2976000</v>
+        <v>1175250</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B51">
-        <v>5406000</v>
+        <v>994500</v>
       </c>
       <c r="C51">
-        <v>4911000</v>
+        <v>977000</v>
       </c>
       <c r="D51">
-        <v>5697000</v>
+        <v>1290500</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B52">
-        <v>420000</v>
+        <v>2209000</v>
       </c>
       <c r="C52">
-        <v>525000</v>
+        <v>1515000</v>
       </c>
       <c r="D52">
-        <v>420000</v>
+        <v>1388000</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B53">
-        <v>135000</v>
+        <v>747840</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>1012480</v>
       </c>
       <c r="D53">
-        <v>45000</v>
+        <v>1416960</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="B54">
-        <v>14500</v>
+        <v>1875000</v>
       </c>
       <c r="C54">
-        <v>11000</v>
+        <v>1385000</v>
       </c>
       <c r="D54">
-        <v>1500</v>
+        <v>1490000</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B55">
-        <v>5675000</v>
+        <v>2249400</v>
       </c>
       <c r="C55">
-        <v>5270000</v>
+        <v>2414600</v>
       </c>
       <c r="D55">
-        <v>6320000</v>
+        <v>1557600</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B56">
-        <v>275000</v>
+        <v>3261000</v>
       </c>
       <c r="C56">
-        <v>365000</v>
+        <v>2840000</v>
       </c>
       <c r="D56">
-        <v>300000</v>
+        <v>1742000</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B57">
-        <v>673000</v>
+        <v>1320000</v>
       </c>
       <c r="C57">
-        <v>879000</v>
+        <v>1600000</v>
       </c>
       <c r="D57">
-        <v>911000</v>
+        <v>1822000</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B58">
-        <v>240000</v>
+        <v>1536000</v>
       </c>
       <c r="C58">
-        <v>480000</v>
+        <v>2122200</v>
       </c>
       <c r="D58">
-        <v>300000</v>
+        <v>1822200</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="B59">
-        <v>6676000</v>
+        <v>1180000</v>
       </c>
       <c r="C59">
-        <v>5680000</v>
+        <v>1562500</v>
       </c>
       <c r="D59">
-        <v>7245000</v>
+        <v>1852500</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B60">
-        <v>734250</v>
+        <v>1385000</v>
       </c>
       <c r="C60">
-        <v>800250</v>
+        <v>1435000</v>
       </c>
       <c r="D60">
-        <v>1175250</v>
+        <v>1925000</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B61">
-        <v>132000</v>
+        <v>1454000</v>
       </c>
       <c r="C61">
-        <v>181500</v>
+        <v>1067000</v>
       </c>
       <c r="D61">
-        <v>115500</v>
+        <v>1946000</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B62">
-        <v>702300</v>
+        <v>1385000</v>
       </c>
       <c r="C62">
-        <v>852500</v>
+        <v>1680000</v>
       </c>
       <c r="D62">
-        <v>966600</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="B63">
-        <v>1680000</v>
+        <v>2464000</v>
       </c>
       <c r="C63">
-        <v>3530000</v>
+        <v>2108000</v>
       </c>
       <c r="D63">
-        <v>2550000</v>
+        <v>2116000</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B64">
-        <v>6215000</v>
+        <v>2095500</v>
       </c>
       <c r="C64">
-        <v>6635000</v>
+        <v>1955500</v>
       </c>
       <c r="D64">
-        <v>6580000</v>
+        <v>2249500</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B65">
-        <v>6000</v>
+        <v>1680000</v>
       </c>
       <c r="C65">
-        <v>1500</v>
+        <v>3530000</v>
       </c>
       <c r="D65">
-        <v>1500</v>
+        <v>2550000</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B66">
-        <v>9089500</v>
+        <v>2794000</v>
       </c>
       <c r="C66">
-        <v>8449900</v>
+        <v>2262000</v>
       </c>
       <c r="D66">
-        <v>8854100</v>
+        <v>2976000</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B67">
-        <v>2095500</v>
+        <v>4332000</v>
       </c>
       <c r="C67">
-        <v>1955500</v>
+        <v>5039000</v>
       </c>
       <c r="D67">
-        <v>2249500</v>
+        <v>3470000</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="B68">
-        <v>747840</v>
+        <v>5210000</v>
       </c>
       <c r="C68">
-        <v>1012480</v>
+        <v>4286000</v>
       </c>
       <c r="D68">
-        <v>1416960</v>
+        <v>4105000</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="B69">
-        <v>5447500</v>
+        <v>5401000</v>
       </c>
       <c r="C69">
-        <v>5615900</v>
+        <v>5642000</v>
       </c>
       <c r="D69">
-        <v>5942600</v>
+        <v>4642000</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="B70">
-        <v>30000</v>
+        <v>3655000</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>4084000</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>5032000</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B71">
-        <v>16500</v>
+        <v>5353000</v>
       </c>
       <c r="C71">
-        <v>37500</v>
+        <v>6744000</v>
       </c>
       <c r="D71">
-        <v>20000</v>
+        <v>5215000</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>3048000</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>5020000</v>
       </c>
       <c r="D72">
-        <v>30000</v>
+        <v>5242000</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="B73">
-        <v>72000</v>
+        <v>5406000</v>
       </c>
       <c r="C73">
-        <v>105000</v>
+        <v>4911000</v>
       </c>
       <c r="D73">
-        <v>164000</v>
+        <v>5697000</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>3392000</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>4281000</v>
       </c>
       <c r="D74">
-        <v>400000</v>
+        <v>5830000</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B75">
-        <v>48000</v>
+        <v>5447500</v>
       </c>
       <c r="C75">
-        <v>45000</v>
+        <v>5615900</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>5942600</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="B76">
-        <v>1385000</v>
+        <v>7248000</v>
       </c>
       <c r="C76">
-        <v>1435000</v>
+        <v>3889000</v>
       </c>
       <c r="D76">
-        <v>1925000</v>
+        <v>6227000</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B77">
-        <v>1385000</v>
+        <v>5675000</v>
       </c>
       <c r="C77">
-        <v>1680000</v>
+        <v>5270000</v>
       </c>
       <c r="D77">
-        <v>2000000</v>
+        <v>6320000</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B78">
-        <v>92000</v>
+        <v>6215000</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>6635000</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>6580000</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B79">
-        <v>3392000</v>
+        <v>4197000</v>
       </c>
       <c r="C79">
-        <v>4281000</v>
+        <v>6320000</v>
       </c>
       <c r="D79">
-        <v>5830000</v>
+        <v>6906000</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B80">
-        <v>190000</v>
+        <v>6676000</v>
       </c>
       <c r="C80">
-        <v>220000</v>
+        <v>5680000</v>
       </c>
       <c r="D80">
-        <v>495000</v>
+        <v>7245000</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="B81">
-        <v>1454000</v>
+        <v>10682000</v>
       </c>
       <c r="C81">
-        <v>1067000</v>
+        <v>9214000</v>
       </c>
       <c r="D81">
-        <v>1946000</v>
+        <v>8703000</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B82">
-        <v>4197000</v>
+        <v>9089500</v>
       </c>
       <c r="C82">
-        <v>6320000</v>
+        <v>8449900</v>
       </c>
       <c r="D82">
-        <v>6906000</v>
+        <v>8854100</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B83">
-        <v>400000</v>
+        <v>9591000</v>
       </c>
       <c r="C83">
-        <v>240000</v>
+        <v>9055000</v>
       </c>
       <c r="D83">
-        <v>560000</v>
+        <v>9600000</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="B84">
-        <v>2270000</v>
+        <v>13058000</v>
       </c>
       <c r="C84">
-        <v>1605000</v>
+        <v>11589000</v>
       </c>
       <c r="D84">
-        <v>555000</v>
+        <v>11844000</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="B85">
-        <v>730000</v>
+        <v>11656000</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>11001000</v>
       </c>
       <c r="D85">
-        <v>390000</v>
+        <v>12364000</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="B86">
-        <v>4332000</v>
+        <v>12683000</v>
       </c>
       <c r="C86">
-        <v>5039000</v>
+        <v>13015000</v>
       </c>
       <c r="D86">
-        <v>3470000</v>
+        <v>13890000</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="B87">
-        <v>9591000</v>
+        <v>21522000</v>
       </c>
       <c r="C87">
-        <v>9055000</v>
+        <v>18687000</v>
       </c>
       <c r="D87">
-        <v>9600000</v>
+        <v>20505000</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="B88">
-        <v>60000</v>
+        <v>25182000</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>24248000</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>24172000</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="B89">
-        <v>53932000</v>
+        <v>39934000</v>
       </c>
       <c r="C89">
-        <v>40276000</v>
+        <v>38194000</v>
       </c>
       <c r="D89">
-        <v>50066000</v>
+        <v>39205000</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="B90">
-        <v>6000</v>
+        <v>39003000</v>
       </c>
       <c r="C90">
-        <v>15000</v>
+        <v>41119000</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>40209000</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B91">
-        <v>10000</v>
+        <v>53932000</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>40276000</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>50066000</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D91">
+    <sortCondition ref="D2:D91"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>